<commit_message>
Answers exam 1 - v2, and class exercises in Python
</commit_message>
<xml_diff>
--- a/Clase 7 - parcial/Solución parcial/Solucionario_parcial.xlsx
+++ b/Clase 7 - parcial/Solución parcial/Solucionario_parcial.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\OneDrive\Desktop\Clases-Eafit\Introduccion-a-la-programacion\Clase 7 - parcial\Solución parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76458EF9-0FFA-462B-8732-136351D758F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E1C270-C43F-4D70-9932-DF6EC78028C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57CED19C-FBAE-4BAF-9BD4-DB6925AA300D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{57CED19C-FBAE-4BAF-9BD4-DB6925AA300D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parcial 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parcial 1 _ version 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="29">
   <si>
     <t>Pregunta 1</t>
   </si>
@@ -109,6 +110,18 @@
   </si>
   <si>
     <t>(~pv~q)^q</t>
+  </si>
+  <si>
+    <t>Diagrama de flujo</t>
+  </si>
+  <si>
+    <t>(p^¬q)v¬p</t>
+  </si>
+  <si>
+    <t>(¬pv¬q)^q</t>
+  </si>
+  <si>
+    <t>(p^¬q)</t>
   </si>
 </sst>
 </file>
@@ -501,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7435326C-AB19-4C5F-99A7-7BCDAA559E9B}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,16 +770,300 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840F08C0-7D8A-4DAA-B32A-10B8C7A96BC6}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007430196D5E630441B6F9955AF8B8AB7E" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="7f230af0e932d6b16252d51b0a9260b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eca7645dcb7ed048c116615a1929d1db">
     <xsd:element name="properties">
@@ -880,6 +1177,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -887,14 +1193,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7BB9BCF-3F7E-44AA-A2A6-E8D63CCCEACE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7237F5B8-41A4-4825-BBB9-E390B3DE6033}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -906,6 +1204,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7BB9BCF-3F7E-44AA-A2A6-E8D63CCCEACE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>